<commit_message>
Forgot to update this
</commit_message>
<xml_diff>
--- a/images/Wealth tax graph.xlsx
+++ b/images/Wealth tax graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeemi\OneDrive\Documents\GitHub\PhillyTechDudeBro69\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC225EF9-F021-4F81-86E9-D6799E4A2C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907428D-24FE-4D29-9A68-4AD5B84022C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F02010A-BE7A-4D82-8038-497F747FAB63}"/>
   </bookViews>
@@ -7422,7 +7422,7 @@
   <dimension ref="A1:B1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>